<commit_message>
last fix in the data
</commit_message>
<xml_diff>
--- a/Stomach.content.all.xlsx
+++ b/Stomach.content.all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/510852ff01b61d64/Documentos/Czech Phd/R/stomach_content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="14_{35A09E31-ECEC-40D6-8DBC-C44FDA68393F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{623F06C4-B2CD-4D73-85C7-8CC093E5DE9C}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="14_{35A09E31-ECEC-40D6-8DBC-C44FDA68393F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F640F7B-3225-496F-AB53-D1866D924013}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2970" windowWidth="29040" windowHeight="15840" xr2:uid="{FF613A98-EB61-4E1B-BAB3-1C94EAABA9AC}"/>
+    <workbookView xWindow="7488" yWindow="6804" windowWidth="11076" windowHeight="6000" activeTab="1" xr2:uid="{FF613A98-EB61-4E1B-BAB3-1C94EAABA9AC}"/>
   </bookViews>
   <sheets>
     <sheet name="stomach" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">candat!$E$1:$E$593</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">stomach!$A$1:$BQ$910</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">stomach!$A$1:$BQ$909</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -599,6 +599,10 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
+<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -896,11 +900,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03FF9E8A-144A-4DD1-84C5-0292E9791074}">
-  <dimension ref="A1:BQ911"/>
+  <dimension ref="A1:BQ910"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A878" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M910" sqref="M910:AC910"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A906" sqref="A906:XFD906"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -54543,18 +54547,36 @@
       <c r="BQ905" s="1"/>
     </row>
     <row r="906" spans="1:69" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A906" s="1"/>
-      <c r="B906" s="1"/>
-      <c r="C906" s="2"/>
-      <c r="D906" s="1"/>
+      <c r="A906" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B906" s="3">
+        <v>40423</v>
+      </c>
+      <c r="C906" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D906" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="E906" s="1"/>
       <c r="F906" s="1"/>
-      <c r="G906" s="1"/>
-      <c r="H906" s="1"/>
+      <c r="G906" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H906" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="I906" s="1"/>
-      <c r="J906" s="1"/>
-      <c r="K906" s="1"/>
-      <c r="L906" s="1"/>
+      <c r="J906" s="1">
+        <v>250</v>
+      </c>
+      <c r="K906" s="7">
+        <v>188</v>
+      </c>
+      <c r="L906" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="M906" s="1">
         <v>0</v>
       </c>
@@ -54574,8 +54596,7 @@
       <c r="AA906" s="1"/>
       <c r="AB906" s="1"/>
       <c r="AC906" s="1">
-        <f>SUM(AD906:BQ906)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD906" s="1"/>
       <c r="AE906" s="1"/>
@@ -54612,7 +54633,9 @@
       <c r="BJ906" s="1"/>
       <c r="BK906" s="1"/>
       <c r="BL906" s="1"/>
-      <c r="BM906" s="1"/>
+      <c r="BM906" s="1">
+        <v>1</v>
+      </c>
       <c r="BN906" s="1"/>
       <c r="BO906" s="1"/>
       <c r="BP906" s="1"/>
@@ -54623,28 +54646,34 @@
         <v>2010</v>
       </c>
       <c r="B907" s="3">
-        <v>40423</v>
+        <v>40421</v>
       </c>
       <c r="C907" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D907" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E907" s="1"/>
-      <c r="F907" s="1"/>
+      <c r="E907" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F907" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="G907" s="1" t="s">
-        <v>26</v>
+        <v>98</v>
       </c>
       <c r="H907" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I907" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="I907" s="1">
+        <v>45284</v>
+      </c>
       <c r="J907" s="1">
-        <v>250</v>
+        <v>135</v>
       </c>
       <c r="K907" s="7">
-        <v>188</v>
+        <v>37</v>
       </c>
       <c r="L907" s="1" t="s">
         <v>57</v>
@@ -54668,7 +54697,7 @@
       <c r="AA907" s="1"/>
       <c r="AB907" s="1"/>
       <c r="AC907" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD907" s="1"/>
       <c r="AE907" s="1"/>
@@ -54705,9 +54734,7 @@
       <c r="BJ907" s="1"/>
       <c r="BK907" s="1"/>
       <c r="BL907" s="1"/>
-      <c r="BM907" s="1">
-        <v>1</v>
-      </c>
+      <c r="BM907" s="1"/>
       <c r="BN907" s="1"/>
       <c r="BO907" s="1"/>
       <c r="BP907" s="1"/>
@@ -54717,38 +54744,38 @@
       <c r="A908" s="1">
         <v>2010</v>
       </c>
-      <c r="B908" s="3">
-        <v>40421</v>
+      <c r="B908" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C908" s="2" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="D908" s="1" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="E908" s="1" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="F908" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="G908" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H908" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="I908" s="1">
-        <v>45284</v>
+        <v>738875</v>
       </c>
       <c r="J908" s="1">
-        <v>135</v>
+        <v>400</v>
       </c>
       <c r="K908" s="7">
-        <v>37</v>
+        <v>791.23450000000003</v>
       </c>
       <c r="L908" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M908" s="1">
         <v>0</v>
@@ -54769,7 +54796,7 @@
       <c r="AA908" s="1"/>
       <c r="AB908" s="1"/>
       <c r="AC908" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD908" s="1"/>
       <c r="AE908" s="1"/>
@@ -54806,45 +54833,47 @@
       <c r="BJ908" s="1"/>
       <c r="BK908" s="1"/>
       <c r="BL908" s="1"/>
-      <c r="BM908" s="1"/>
+      <c r="BM908" s="1">
+        <v>1</v>
+      </c>
       <c r="BN908" s="1"/>
       <c r="BO908" s="1"/>
       <c r="BP908" s="1"/>
       <c r="BQ908" s="1"/>
     </row>
-    <row r="909" spans="1:69" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="909" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A909" s="1">
         <v>2010</v>
       </c>
-      <c r="B909" s="3" t="s">
-        <v>48</v>
+      <c r="B909" s="3">
+        <v>40421</v>
       </c>
       <c r="C909" s="2" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="D909" s="1" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="E909" s="1" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="F909" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G909" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H909" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="I909" s="1">
-        <v>738875</v>
+        <v>45406</v>
       </c>
       <c r="J909" s="1">
-        <v>400</v>
+        <v>175</v>
       </c>
       <c r="K909" s="7">
-        <v>791.23450000000003</v>
+        <v>105</v>
       </c>
       <c r="L909" s="1" t="s">
         <v>58</v>
@@ -54852,122 +54881,21 @@
       <c r="M909" s="1">
         <v>0</v>
       </c>
-      <c r="N909" s="1"/>
-      <c r="O909" s="1"/>
-      <c r="P909" s="1"/>
-      <c r="Q909" s="1"/>
-      <c r="R909" s="1"/>
-      <c r="S909" s="1"/>
-      <c r="T909" s="1"/>
-      <c r="U909" s="1"/>
-      <c r="V909" s="1"/>
-      <c r="W909" s="1"/>
-      <c r="X909" s="1"/>
-      <c r="Y909" s="1"/>
-      <c r="Z909" s="1"/>
-      <c r="AA909" s="1"/>
-      <c r="AB909" s="1"/>
       <c r="AC909" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD909" s="1"/>
-      <c r="AE909" s="1"/>
-      <c r="AF909" s="1"/>
-      <c r="AG909" s="1"/>
-      <c r="AH909" s="1"/>
-      <c r="AI909" s="1"/>
-      <c r="AJ909" s="1"/>
-      <c r="AK909" s="1"/>
-      <c r="AL909" s="1"/>
-      <c r="AM909" s="1"/>
-      <c r="AN909" s="1"/>
-      <c r="AO909" s="1"/>
-      <c r="AP909" s="1"/>
-      <c r="AQ909" s="1"/>
-      <c r="AR909" s="1"/>
-      <c r="AS909" s="1"/>
-      <c r="AT909" s="1"/>
-      <c r="AU909" s="1"/>
-      <c r="AV909" s="1"/>
-      <c r="AW909" s="1"/>
-      <c r="AX909" s="1"/>
-      <c r="AY909" s="1"/>
-      <c r="AZ909" s="1"/>
-      <c r="BA909" s="1"/>
-      <c r="BB909" s="1"/>
-      <c r="BC909" s="1"/>
-      <c r="BD909" s="1"/>
-      <c r="BE909" s="1"/>
-      <c r="BF909" s="1"/>
-      <c r="BG909" s="1"/>
-      <c r="BH909" s="1"/>
-      <c r="BI909" s="1"/>
-      <c r="BJ909" s="1"/>
-      <c r="BK909" s="1"/>
-      <c r="BL909" s="1"/>
-      <c r="BM909" s="1">
-        <v>1</v>
-      </c>
-      <c r="BN909" s="1"/>
-      <c r="BO909" s="1"/>
-      <c r="BP909" s="1"/>
-      <c r="BQ909" s="1"/>
+        <f>SUM(AC2:AC908)</f>
+        <v>418</v>
+      </c>
     </row>
     <row r="910" spans="1:69" x14ac:dyDescent="0.3">
-      <c r="A910" s="1">
-        <v>2010</v>
-      </c>
-      <c r="B910" s="3">
-        <v>40421</v>
-      </c>
-      <c r="C910" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D910" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E910" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F910" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G910" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H910" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I910" s="1">
-        <v>45406</v>
-      </c>
-      <c r="J910" s="1">
-        <v>175</v>
-      </c>
-      <c r="K910" s="7">
-        <v>105</v>
-      </c>
-      <c r="L910" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="M910" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC910" s="1">
-        <f>SUM(AC2:AC909)</f>
-        <v>418</v>
-      </c>
-    </row>
-    <row r="911" spans="1:69" x14ac:dyDescent="0.3">
-      <c r="M911" s="1">
-        <f>SUM(M2:M910)</f>
+        <f>SUM(M2:M909)</f>
         <v>637</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BQ910" xr:uid="{03FF9E8A-144A-4DD1-84C5-0292E9791074}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:BQ910">
-      <sortCondition descending="1" ref="AC1:AC909"/>
+  <autoFilter ref="A1:BQ909" xr:uid="{03FF9E8A-144A-4DD1-84C5-0292E9791074}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:BQ909">
+      <sortCondition descending="1" ref="AC1:AC908"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -54980,9 +54908,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B6C920-462B-4125-844F-0115D5AB452B}">
   <dimension ref="A1:BG876"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E316" sqref="E316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>